<commit_message>
need to fix A_leader_follower
</commit_message>
<xml_diff>
--- a/GroupElementListCx1.xlsx
+++ b/GroupElementListCx1.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -699,199 +699,2016 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>1.865</t>
+          <t>1.550</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>Inflatable Gasket</t>
+          <t>Exhaust air flap</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>S_GASKET</t>
+          <t>S_MOTOR1</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G8" t="n">
-        <v>1.865</v>
+        <v>1.55</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>['PSA-', 'V']</t>
+          <t>['GIA', 'K', 'Y', 'YC']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>1.866</t>
+          <t>1.555</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>Inflatable Gasket</t>
+          <t>Exhaust bypass valve</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>S_GASKET</t>
+          <t>S_MOTOR1</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>1.866</v>
+        <v>1.555</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>['PSA-', 'V']</t>
+          <t>['GIA', 'V', 'Y', 'YC']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="n">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>1.867</t>
+          <t>1.560</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>Inflatable Gasket</t>
+          <t>Exhaust air flap</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>S_GASKET</t>
+          <t>S_MOTOR1</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G10" t="n">
-        <v>1.867</v>
+        <v>1.56</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>['PSA-', 'V']</t>
+          <t>['GIA', 'K', 'Y', 'YC']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="n">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>1.868</t>
+          <t>1.655</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>Inflatable Gasket</t>
+          <t>Control valve</t>
         </is>
       </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>S_GASKET</t>
+          <t>S_MOTOR1</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G11" t="n">
-        <v>1.868</v>
+        <v>1.655</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>['PSA-', 'V']</t>
+          <t>['H', 'M', 'NC']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="C12" s="1" t="inlineStr">
-        <is>
-          <t>1.869</t>
-        </is>
-      </c>
-      <c r="D12" s="1" t="inlineStr">
-        <is>
-          <t>Inflatable Gasket</t>
-        </is>
-      </c>
+      <c r="B12" s="1" t="n"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="1" t="n"/>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>S_GASKET</t>
+          <t>S_REG_CONT</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G12" t="n">
-        <v>1.869</v>
+        <v>1.655</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>['PSA-', 'V']</t>
+          <t>['H', 'M', 'NC']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="1" t="n"/>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>1.680</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>Electric heating</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>S_MOTOR1</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>['EC', 'TSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="1" t="n"/>
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="1" t="n"/>
+      <c r="E14" s="1" t="inlineStr">
+        <is>
+          <t>S_REG_CONT</t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>['EC', 'TSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>1.800</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>Temperature sensor</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>['TICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="1" t="n"/>
+      <c r="C16" s="1" t="n"/>
+      <c r="D16" s="1" t="n"/>
+      <c r="E16" s="1" t="n"/>
+      <c r="F16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>['TICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>1.690</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>Dryer / Humidifier</t>
+        </is>
+      </c>
+      <c r="E17" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_ON_OFF</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>['T', 'XA']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="1" t="n"/>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>1.810</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>Humidity sensor</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>['MIA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="n"/>
+      <c r="C19" s="1" t="n"/>
+      <c r="D19" s="1" t="n"/>
+      <c r="E19" s="1" t="n"/>
+      <c r="F19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>['MIA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>1.815</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>Weight scale</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1.815</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="1" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="inlineStr">
+        <is>
+          <t>S_WEIGHT_SCALE2_NG</t>
+        </is>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1.815</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n"/>
+      <c r="B22" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>1.816</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>Weight scale</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.816</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="n"/>
+      <c r="C23" s="1" t="n"/>
+      <c r="D23" s="1" t="n"/>
+      <c r="E23" s="1" t="inlineStr">
+        <is>
+          <t>S_WEIGHT_SCALE2_NG</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.816</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>1.830</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>H2O2 LC sensor</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_SWITCH</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'QIA+', 'XA']</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n"/>
+      <c r="B25" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>1.865</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>Inflatable Gasket</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>S_GASKET</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1.865</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>['PSA-', 'V']</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n"/>
+      <c r="B26" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>1.866</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>Inflatable Gasket</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>S_GASKET</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1.866</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>['PSA-', 'V']</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t>1.867</t>
+        </is>
+      </c>
+      <c r="D27" s="1" t="inlineStr">
+        <is>
+          <t>Inflatable Gasket</t>
+        </is>
+      </c>
+      <c r="E27" s="1" t="inlineStr">
+        <is>
+          <t>S_GASKET</t>
+        </is>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1.867</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>['PSA-', 'V']</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n"/>
+      <c r="B28" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>1.868</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>Inflatable Gasket</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>S_GASKET</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.868</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>['PSA-', 'V']</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n"/>
+      <c r="B29" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>1.869</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>Inflatable Gasket</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>S_GASKET</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.869</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>['PSA-', 'V']</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n"/>
+      <c r="B30" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="C13" s="1" t="inlineStr">
+      <c r="C30" s="1" t="inlineStr">
         <is>
           <t>1.870</t>
         </is>
       </c>
-      <c r="D13" s="1" t="inlineStr">
+      <c r="D30" s="1" t="inlineStr">
         <is>
           <t>Inflatable Gasket</t>
         </is>
       </c>
-      <c r="E13" s="1" t="inlineStr">
+      <c r="E30" s="1" t="inlineStr">
         <is>
           <t>S_GASKET</t>
         </is>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F30" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G30" t="n">
         <v>1.87</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>['PSA-', 'V']</t>
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_ON_OFF</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>1.690</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>Dryer / Humidifier</t>
+        </is>
+      </c>
+      <c r="E31" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>['T', 'XA']</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_SWITCH</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>1.725</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="inlineStr">
+        <is>
+          <t>Flow Switch H2O2</t>
+        </is>
+      </c>
+      <c r="E32" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1.725</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>['LSA-']</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n"/>
+      <c r="B33" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>1.830</t>
+        </is>
+      </c>
+      <c r="D33" s="1" t="inlineStr">
+        <is>
+          <t>H2O2 LC sensor</t>
+        </is>
+      </c>
+      <c r="E33" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'QIA+', 'XA']</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n"/>
+      <c r="B34" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="inlineStr">
+        <is>
+          <t>1.833</t>
+        </is>
+      </c>
+      <c r="D34" s="1" t="inlineStr">
+        <is>
+          <t>TLV H2O2 LC Sensor</t>
+        </is>
+      </c>
+      <c r="E34" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_SWITCH</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1.833</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>['QSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n"/>
+      <c r="B35" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1" t="inlineStr">
+        <is>
+          <t>1.833</t>
+        </is>
+      </c>
+      <c r="D35" s="1" t="inlineStr">
+        <is>
+          <t>TLV H2O2 LC Sensor</t>
+        </is>
+      </c>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_SWITCH</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1.833</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>['QSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n"/>
+      <c r="B36" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C36" s="1" t="inlineStr">
+        <is>
+          <t>1.834</t>
+        </is>
+      </c>
+      <c r="D36" s="1" t="inlineStr">
+        <is>
+          <t>TLV H2O2 LC Sensor</t>
+        </is>
+      </c>
+      <c r="E36" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_SWITCH</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1.834</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>['QSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n"/>
+      <c r="B37" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C37" s="1" t="inlineStr">
+        <is>
+          <t>1.834</t>
+        </is>
+      </c>
+      <c r="D37" s="1" t="inlineStr">
+        <is>
+          <t>TLV H2O2 LC Sensor</t>
+        </is>
+      </c>
+      <c r="E37" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_SWITCH</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1.834</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>['QSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>S_MOTOR1</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C38" s="1" t="inlineStr">
+        <is>
+          <t>1.550</t>
+        </is>
+      </c>
+      <c r="D38" s="1" t="inlineStr">
+        <is>
+          <t>Exhaust air flap</t>
+        </is>
+      </c>
+      <c r="E38" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>['GIA', 'K', 'Y', 'YC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n"/>
+      <c r="B39" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="C39" s="1" t="inlineStr">
+        <is>
+          <t>1.555</t>
+        </is>
+      </c>
+      <c r="D39" s="1" t="inlineStr">
+        <is>
+          <t>Exhaust bypass valve</t>
+        </is>
+      </c>
+      <c r="E39" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1.555</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>['GIA', 'V', 'Y', 'YC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n"/>
+      <c r="B40" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>1.560</t>
+        </is>
+      </c>
+      <c r="D40" s="1" t="inlineStr">
+        <is>
+          <t>Exhaust air flap</t>
+        </is>
+      </c>
+      <c r="E40" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F40" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>['GIA', 'K', 'Y', 'YC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n"/>
+      <c r="B41" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>1.655</t>
+        </is>
+      </c>
+      <c r="D41" s="1" t="inlineStr">
+        <is>
+          <t>Control valve</t>
+        </is>
+      </c>
+      <c r="E41" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1.655</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>['H', 'M', 'NC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n"/>
+      <c r="B42" s="1" t="n"/>
+      <c r="C42" s="1" t="n"/>
+      <c r="D42" s="1" t="n"/>
+      <c r="E42" s="1" t="inlineStr">
+        <is>
+          <t>S_REG_CONT</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1.655</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>['H', 'M', 'NC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n"/>
+      <c r="B43" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>1.680</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="inlineStr">
+        <is>
+          <t>Electric heating</t>
+        </is>
+      </c>
+      <c r="E43" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>['EC', 'TSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n"/>
+      <c r="B44" s="1" t="n"/>
+      <c r="C44" s="1" t="n"/>
+      <c r="D44" s="1" t="n"/>
+      <c r="E44" s="1" t="inlineStr">
+        <is>
+          <t>S_REG_CONT</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>['EC', 'TSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>S_PUMP_TEST</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>1.700</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n"/>
+      <c r="B46" s="1" t="n"/>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t>1.710</t>
+        </is>
+      </c>
+      <c r="D46" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E46" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n"/>
+      <c r="B47" s="1" t="n"/>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>1.720</t>
+        </is>
+      </c>
+      <c r="D47" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E47" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n"/>
+      <c r="B48" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t>1.730</t>
+        </is>
+      </c>
+      <c r="D48" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E48" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n"/>
+      <c r="B49" s="1" t="n"/>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>1.740</t>
+        </is>
+      </c>
+      <c r="D49" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E49" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F49" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n"/>
+      <c r="B50" s="1" t="n"/>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>1.750</t>
+        </is>
+      </c>
+      <c r="D50" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E50" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F50" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>S_REG_CONT</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>1.655</t>
+        </is>
+      </c>
+      <c r="D51" s="1" t="inlineStr">
+        <is>
+          <t>Control valve</t>
+        </is>
+      </c>
+      <c r="E51" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F51" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1.655</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>['H', 'M', 'NC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n"/>
+      <c r="B52" s="1" t="n"/>
+      <c r="C52" s="1" t="n"/>
+      <c r="D52" s="1" t="n"/>
+      <c r="E52" s="1" t="inlineStr">
+        <is>
+          <t>S_MOTOR1</t>
+        </is>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1.655</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>['H', 'M', 'NC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n"/>
+      <c r="B53" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t>1.680</t>
+        </is>
+      </c>
+      <c r="D53" s="1" t="inlineStr">
+        <is>
+          <t>Electric heating</t>
+        </is>
+      </c>
+      <c r="E53" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F53" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>['EC', 'TSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n"/>
+      <c r="B54" s="1" t="n"/>
+      <c r="C54" s="1" t="n"/>
+      <c r="D54" s="1" t="n"/>
+      <c r="E54" s="1" t="inlineStr">
+        <is>
+          <t>S_MOTOR1</t>
+        </is>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>['EC', 'TSA+']</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t>1.700</t>
+        </is>
+      </c>
+      <c r="D55" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E55" s="1" t="inlineStr">
+        <is>
+          <t>S_PUMP_TEST</t>
+        </is>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n"/>
+      <c r="B56" s="1" t="n"/>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t>1.710</t>
+        </is>
+      </c>
+      <c r="D56" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E56" s="1" t="inlineStr">
+        <is>
+          <t>S_PUMP_TEST</t>
+        </is>
+      </c>
+      <c r="F56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n"/>
+      <c r="B57" s="1" t="n"/>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t>1.720</t>
+        </is>
+      </c>
+      <c r="D57" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E57" s="1" t="inlineStr">
+        <is>
+          <t>S_PUMP_TEST</t>
+        </is>
+      </c>
+      <c r="F57" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n"/>
+      <c r="B58" s="1" t="n"/>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t>1.725</t>
+        </is>
+      </c>
+      <c r="D58" s="1" t="inlineStr">
+        <is>
+          <t>Flow Switch H2O2</t>
+        </is>
+      </c>
+      <c r="E58" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_SWITCH</t>
+        </is>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1.725</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>['LSA-']</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n"/>
+      <c r="B59" s="1" t="n"/>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t>1.800</t>
+        </is>
+      </c>
+      <c r="D59" s="1" t="inlineStr">
+        <is>
+          <t>Temperature sensor</t>
+        </is>
+      </c>
+      <c r="E59" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>['TICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n"/>
+      <c r="B60" s="1" t="n"/>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t>1.810</t>
+        </is>
+      </c>
+      <c r="D60" s="1" t="inlineStr">
+        <is>
+          <t>Humidity sensor</t>
+        </is>
+      </c>
+      <c r="E60" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>['MIA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n"/>
+      <c r="B61" s="1" t="n"/>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t>1.815</t>
+        </is>
+      </c>
+      <c r="D61" s="1" t="inlineStr">
+        <is>
+          <t>Weight scale</t>
+        </is>
+      </c>
+      <c r="E61" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F61" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1.815</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n"/>
+      <c r="B62" s="1" t="n"/>
+      <c r="C62" s="1" t="n"/>
+      <c r="D62" s="1" t="n"/>
+      <c r="E62" s="1" t="inlineStr">
+        <is>
+          <t>S_WEIGHT_SCALE2_NG</t>
+        </is>
+      </c>
+      <c r="F62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1.815</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n"/>
+      <c r="B63" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1" t="inlineStr">
+        <is>
+          <t>1.730</t>
+        </is>
+      </c>
+      <c r="D63" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E63" s="1" t="inlineStr">
+        <is>
+          <t>S_PUMP_TEST</t>
+        </is>
+      </c>
+      <c r="F63" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n"/>
+      <c r="B64" s="1" t="n"/>
+      <c r="C64" s="1" t="inlineStr">
+        <is>
+          <t>1.740</t>
+        </is>
+      </c>
+      <c r="D64" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E64" s="1" t="inlineStr">
+        <is>
+          <t>S_PUMP_TEST</t>
+        </is>
+      </c>
+      <c r="F64" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n"/>
+      <c r="B65" s="1" t="n"/>
+      <c r="C65" s="1" t="inlineStr">
+        <is>
+          <t>1.750</t>
+        </is>
+      </c>
+      <c r="D65" s="1" t="inlineStr">
+        <is>
+          <t>Peristaltic pump</t>
+        </is>
+      </c>
+      <c r="E65" s="1" t="inlineStr">
+        <is>
+          <t>S_PUMP_TEST</t>
+        </is>
+      </c>
+      <c r="F65" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G65" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>['M', 'P', 'SC']</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n"/>
+      <c r="B66" s="1" t="n"/>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>1.800</t>
+        </is>
+      </c>
+      <c r="D66" s="1" t="inlineStr">
+        <is>
+          <t>Temperature sensor</t>
+        </is>
+      </c>
+      <c r="E66" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F66" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>['TICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n"/>
+      <c r="B67" s="1" t="n"/>
+      <c r="C67" s="1" t="inlineStr">
+        <is>
+          <t>1.810</t>
+        </is>
+      </c>
+      <c r="D67" s="1" t="inlineStr">
+        <is>
+          <t>Humidity sensor</t>
+        </is>
+      </c>
+      <c r="E67" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F67" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>['MIA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n"/>
+      <c r="B68" s="1" t="n"/>
+      <c r="C68" s="1" t="inlineStr">
+        <is>
+          <t>1.816</t>
+        </is>
+      </c>
+      <c r="D68" s="1" t="inlineStr">
+        <is>
+          <t>Weight scale</t>
+        </is>
+      </c>
+      <c r="E68" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F68" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="G68" t="n">
+        <v>1.816</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n"/>
+      <c r="B69" s="1" t="n"/>
+      <c r="C69" s="1" t="n"/>
+      <c r="D69" s="1" t="n"/>
+      <c r="E69" s="1" t="inlineStr">
+        <is>
+          <t>S_WEIGHT_SCALE2_NG</t>
+        </is>
+      </c>
+      <c r="F69" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G69" t="n">
+        <v>1.816</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>S_WEIGHT_SCALE2_NG</t>
+        </is>
+      </c>
+      <c r="B70" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" s="1" t="inlineStr">
+        <is>
+          <t>1.815</t>
+        </is>
+      </c>
+      <c r="D70" s="1" t="inlineStr">
+        <is>
+          <t>Weight scale</t>
+        </is>
+      </c>
+      <c r="E70" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F70" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1.815</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n"/>
+      <c r="B71" s="1" t="n"/>
+      <c r="C71" s="1" t="n"/>
+      <c r="D71" s="1" t="n"/>
+      <c r="E71" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F71" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G71" t="n">
+        <v>1.815</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n"/>
+      <c r="B72" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C72" s="1" t="inlineStr">
+        <is>
+          <t>1.816</t>
+        </is>
+      </c>
+      <c r="D72" s="1" t="inlineStr">
+        <is>
+          <t>Weight scale</t>
+        </is>
+      </c>
+      <c r="E72" s="1" t="inlineStr">
+        <is>
+          <t>S_LIMIT_HI_LO</t>
+        </is>
+      </c>
+      <c r="F72" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="G72" t="n">
+        <v>1.816</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n"/>
+      <c r="B73" s="1" t="n"/>
+      <c r="C73" s="1" t="n"/>
+      <c r="D73" s="1" t="n"/>
+      <c r="E73" s="1" t="inlineStr">
+        <is>
+          <t>S_SIS</t>
+        </is>
+      </c>
+      <c r="F73" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1.816</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>['WICA±']</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="53">
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A8:A30"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="A45:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B62"/>
+    <mergeCell ref="B63:B69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E18:E19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>